<commit_message>
Updated PCB and added Power Distribution Board
</commit_message>
<xml_diff>
--- a/LIST OF COMPONENTS/LIST - 11th October.xlsx
+++ b/LIST OF COMPONENTS/LIST - 11th October.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="122">
   <si>
     <t>Name</t>
   </si>
@@ -278,9 +278,6 @@
     <t>Off Board (TX, RX, 3.3V and 0V)</t>
   </si>
   <si>
-    <t>10k</t>
-  </si>
-  <si>
     <t>HYT-271</t>
   </si>
   <si>
@@ -348,6 +345,51 @@
   </si>
   <si>
     <t>Grub Screws</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/bourns/cr0805-fx-1002elf/resistor-10k-0-125w-1/dp/1612522</t>
+  </si>
+  <si>
+    <t>Break Away Headers - Machine Pin</t>
+  </si>
+  <si>
+    <t>Bourns 10k SMD 0805 Resistor</t>
+  </si>
+  <si>
+    <t>Texas Instruments DRV 8833</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/texas-instruments/drv8833pwpr/ic-motor-driver-stepper-htssop/dp/2057085</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/murata/grm21bc80g107me15l/capacitor-mlcc-x6s-100uf-4v-0805/dp/2494477</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>Murata 100muF capacitor</t>
+  </si>
+  <si>
+    <t>Panasonic 75kOhm Resistor</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/panasonic-electronic-components/erj6geyj753v/resistor-thick-film-75kohm-5-0805/dp/2323867</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TDK 2.2muF </t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/tdk/c2012x7r1h225k125ac/cap-mlcc-x7r-2-2uf-50v-0805/dp/2346945</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kemet 0.01muF </t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/kemet/c0805c103k5ractu/cap-mlcc-x7r-10nf-50v-0805/dp/1414662</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/117</t>
   </si>
 </sst>
 </file>
@@ -357,7 +399,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,14 +418,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -495,12 +529,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -510,12 +543,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -549,11 +579,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -835,10 +866,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -895,7 +926,7 @@
       <c r="E2" s="1">
         <v>6.56</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="1">
@@ -1291,63 +1322,78 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="9"/>
+      <c r="B19" s="29"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>60</v>
       </c>
+      <c r="B21" t="s">
+        <v>108</v>
+      </c>
       <c r="D21" s="4">
         <v>3</v>
       </c>
       <c r="E21" s="1">
-        <v>0.1</v>
+        <v>2.95</v>
+      </c>
+      <c r="F21" t="s">
+        <v>121</v>
       </c>
       <c r="G21" s="1">
         <f>D21*E21</f>
-        <v>0.30000000000000004</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
+        <v>8.8500000000000014</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" t="s">
+        <v>113</v>
+      </c>
+      <c r="D22" s="4">
+        <v>20</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1.2200000000000001E-2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>116</v>
+      </c>
+      <c r="G22" s="1">
+        <f>D22*E22</f>
+        <v>0.24400000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="B23" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D23" s="22">
         <v>20</v>
       </c>
-      <c r="E22" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="G22" s="1">
-        <f t="shared" ref="G22:G48" si="0">D22*E22</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="4">
-        <v>20</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0.1</v>
+      <c r="E23" s="6">
+        <v>0.22</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="G23" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" ref="G23:G47" si="0">D23*E23</f>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -1355,309 +1401,340 @@
         <v>62</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" s="24">
+        <v>63</v>
+      </c>
+      <c r="D24" s="4">
         <v>20</v>
       </c>
       <c r="E24" s="1">
-        <v>0.1</v>
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>107</v>
       </c>
       <c r="G24" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.78400000000000003</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="4">
-        <v>10</v>
+        <v>64</v>
+      </c>
+      <c r="D25" s="23">
+        <v>20</v>
       </c>
       <c r="E25" s="1">
-        <v>0.1</v>
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="F25" t="s">
+        <v>107</v>
       </c>
       <c r="G25" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.78400000000000003</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>59</v>
+        <v>66</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D26" s="4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E26" s="1">
-        <v>0.1</v>
+        <v>2.5</v>
+      </c>
+      <c r="F26" t="s">
+        <v>111</v>
       </c>
       <c r="G26" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>59</v>
       </c>
+      <c r="B27" s="5" t="s">
+        <v>117</v>
+      </c>
       <c r="C27" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D27" s="4">
         <v>20</v>
       </c>
       <c r="E27" s="1">
-        <v>0.1</v>
+        <f>0.37/2</f>
+        <v>0.185</v>
+      </c>
+      <c r="F27" t="s">
+        <v>118</v>
       </c>
       <c r="G27" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" t="s">
-        <v>87</v>
+        <v>59</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D28" s="4">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E28" s="1">
-        <v>13.02</v>
-      </c>
-      <c r="F28" s="30" t="s">
-        <v>103</v>
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>120</v>
       </c>
       <c r="G28" s="1">
         <f t="shared" si="0"/>
-        <v>78.12</v>
+        <v>0.312</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D29" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E29" s="1">
-        <v>26.49</v>
-      </c>
-      <c r="F29" s="30" t="s">
-        <v>93</v>
+        <v>13.02</v>
+      </c>
+      <c r="F29" t="s">
+        <v>102</v>
       </c>
       <c r="G29" s="1">
         <f t="shared" si="0"/>
-        <v>132.44999999999999</v>
+        <v>78.12</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
-      </c>
-      <c r="C30" t="s">
-        <v>72</v>
+        <v>84</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="D30" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E30" s="1">
-        <v>1.84</v>
+        <v>26.49</v>
       </c>
       <c r="F30" t="s">
         <v>92</v>
       </c>
       <c r="G30" s="1">
         <f t="shared" si="0"/>
-        <v>18.400000000000002</v>
+        <v>132.44999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D31" s="4">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E31" s="1">
-        <v>16.28</v>
+        <v>1.84</v>
       </c>
       <c r="F31" t="s">
         <v>91</v>
       </c>
       <c r="G31" s="1">
         <f t="shared" si="0"/>
+        <v>18.400000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="4">
+        <v>3</v>
+      </c>
+      <c r="E32" s="1">
+        <v>16.28</v>
+      </c>
+      <c r="F32" t="s">
+        <v>90</v>
+      </c>
+      <c r="G32" s="1">
+        <f t="shared" si="0"/>
         <v>48.84</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B34" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" s="24">
+        <v>3</v>
+      </c>
+      <c r="E34" s="11">
+        <v>32.590000000000003</v>
+      </c>
+      <c r="F34" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C33" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D33" s="25">
-        <v>3</v>
-      </c>
-      <c r="E33" s="12">
-        <v>32.590000000000003</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="G33" s="12">
+      <c r="G34" s="11">
         <f t="shared" si="0"/>
         <v>97.77000000000001</v>
       </c>
-      <c r="H33" s="11"/>
-      <c r="I33" s="13"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="14" t="s">
+      <c r="H34" s="10"/>
+      <c r="I34" s="12"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B35" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D35" s="25">
+        <v>3</v>
+      </c>
+      <c r="E35" s="15">
+        <v>6.49</v>
+      </c>
+      <c r="F35" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C34" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="D34" s="26">
-        <v>3</v>
-      </c>
-      <c r="E34" s="16">
-        <v>6.49</v>
-      </c>
-      <c r="F34" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="G34" s="16">
+      <c r="G35" s="15">
         <f t="shared" si="0"/>
         <v>19.47</v>
       </c>
-      <c r="H34" s="15"/>
-      <c r="I34" s="17"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="18" t="s">
+      <c r="H35" s="14"/>
+      <c r="I35" s="16"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="27">
+      <c r="B36" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="26">
         <v>5</v>
       </c>
-      <c r="E35" s="20">
+      <c r="E36" s="19">
         <v>0.98</v>
       </c>
-      <c r="F35" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="G35" s="20">
+      <c r="F36" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>4.9000000000000004</v>
       </c>
-      <c r="H35" s="19"/>
-      <c r="I35" s="21"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>75</v>
-      </c>
-      <c r="D36" s="4">
-        <v>4</v>
-      </c>
+      <c r="H36" s="18"/>
+      <c r="I36" s="20"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>82</v>
       </c>
-      <c r="B37" t="s">
-        <v>94</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="B38" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" t="s">
         <v>83</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D38" s="4">
         <v>5</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E38" s="1">
         <v>16.28</v>
       </c>
-      <c r="F37" t="s">
-        <v>96</v>
-      </c>
-      <c r="G37" s="1">
+      <c r="F38" t="s">
+        <v>95</v>
+      </c>
+      <c r="G38" s="1">
         <f t="shared" si="0"/>
         <v>81.400000000000006</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="B39" s="28"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>89</v>
-      </c>
-      <c r="D41" s="4">
-        <v>10</v>
-      </c>
-      <c r="E41" s="1">
-        <v>2</v>
-      </c>
-      <c r="G41" s="1">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="27"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D42" s="4">
         <v>10</v>
@@ -1670,61 +1747,76 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D44" s="4">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" s="4">
+        <v>10</v>
+      </c>
+      <c r="E43" s="1">
+        <v>2</v>
+      </c>
+      <c r="G43" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D45" s="4">
         <v>3</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E45" s="1">
         <v>50</v>
       </c>
-      <c r="G44" s="1">
+      <c r="G45" s="1">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47" t="s">
         <v>105</v>
       </c>
-      <c r="B46" t="s">
-        <v>106</v>
-      </c>
-      <c r="D46" s="4">
+      <c r="D47" s="4">
         <v>4</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E47" s="1">
         <v>40</v>
       </c>
-      <c r="G46" s="1">
+      <c r="G47" s="1">
         <f t="shared" si="0"/>
         <v>160</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B47" t="s">
-        <v>107</v>
-      </c>
-      <c r="D47" s="4">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>106</v>
+      </c>
+      <c r="D48" s="4">
         <v>2</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E48" s="1">
         <v>3</v>
       </c>
-      <c r="G47" s="1">
-        <f>D47*E47</f>
+      <c r="G48" s="1">
+        <f>D48*E48</f>
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="7" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="29">
-        <f>SUM(G2:G63)</f>
-        <v>1203.7</v>
+      <c r="B52" s="28">
+        <f>SUM(G2:G64)</f>
+        <v>1236.4739999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1732,23 +1824,20 @@
     <mergeCell ref="A19:B19"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F5" r:id="rId4"/>
-    <hyperlink ref="F7" r:id="rId5"/>
-    <hyperlink ref="F8" r:id="rId6"/>
-    <hyperlink ref="F9" r:id="rId7"/>
-    <hyperlink ref="F11" r:id="rId8"/>
-    <hyperlink ref="F12" r:id="rId9"/>
-    <hyperlink ref="F14" r:id="rId10"/>
-    <hyperlink ref="F15" r:id="rId11"/>
-    <hyperlink ref="F16" r:id="rId12"/>
-    <hyperlink ref="F17" r:id="rId13"/>
-    <hyperlink ref="F28" r:id="rId14"/>
-    <hyperlink ref="F29" r:id="rId15"/>
+    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="F4" r:id="rId2"/>
+    <hyperlink ref="F5" r:id="rId3"/>
+    <hyperlink ref="F7" r:id="rId4"/>
+    <hyperlink ref="F8" r:id="rId5"/>
+    <hyperlink ref="F9" r:id="rId6"/>
+    <hyperlink ref="F11" r:id="rId7"/>
+    <hyperlink ref="F12" r:id="rId8"/>
+    <hyperlink ref="F14" r:id="rId9"/>
+    <hyperlink ref="F15" r:id="rId10"/>
+    <hyperlink ref="F16" r:id="rId11"/>
+    <hyperlink ref="F17" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId16"/>
+  <pageSetup paperSize="9" scale="64" orientation="landscape" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated list of components with PCB references
</commit_message>
<xml_diff>
--- a/LIST OF COMPONENTS/LIST - 11th October.xlsx
+++ b/LIST OF COMPONENTS/LIST - 11th October.xlsx
@@ -868,8 +868,8 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1335,7 +1335,7 @@
         <v>108</v>
       </c>
       <c r="D21" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E21" s="1">
         <v>2.95</v>
@@ -1345,7 +1345,7 @@
       </c>
       <c r="G21" s="1">
         <f>D21*E21</f>
-        <v>8.8500000000000014</v>
+        <v>14.75</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -1359,7 +1359,7 @@
         <v>113</v>
       </c>
       <c r="D22" s="4">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E22" s="1">
         <v>1.2200000000000001E-2</v>
@@ -1369,7 +1369,7 @@
       </c>
       <c r="G22" s="1">
         <f>D22*E22</f>
-        <v>0.24400000000000002</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1383,7 +1383,7 @@
         <v>61</v>
       </c>
       <c r="D23" s="22">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E23" s="6">
         <v>0.22</v>
@@ -1393,7 +1393,7 @@
       </c>
       <c r="G23" s="1">
         <f t="shared" ref="G23:G47" si="0">D23*E23</f>
-        <v>4.4000000000000004</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -1407,7 +1407,7 @@
         <v>63</v>
       </c>
       <c r="D24" s="4">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E24" s="1">
         <v>3.9199999999999999E-2</v>
@@ -1417,7 +1417,7 @@
       </c>
       <c r="G24" s="1">
         <f t="shared" si="0"/>
-        <v>0.78400000000000003</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -1431,7 +1431,7 @@
         <v>64</v>
       </c>
       <c r="D25" s="23">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E25" s="1">
         <v>3.9199999999999999E-2</v>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="G25" s="1">
         <f t="shared" si="0"/>
-        <v>0.78400000000000003</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -1479,7 +1479,7 @@
         <v>67</v>
       </c>
       <c r="D27" s="4">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E27" s="1">
         <f>0.37/2</f>
@@ -1490,7 +1490,7 @@
       </c>
       <c r="G27" s="1">
         <f t="shared" si="0"/>
-        <v>3.7</v>
+        <v>9.25</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1504,7 +1504,7 @@
         <v>68</v>
       </c>
       <c r="D28" s="4">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E28" s="1">
         <v>1.5599999999999999E-2</v>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="G28" s="1">
         <f t="shared" si="0"/>
-        <v>0.312</v>
+        <v>0.77999999999999992</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="B52" s="28">
         <f>SUM(G2:G64)</f>
-        <v>1236.4739999999999</v>
+        <v>1257.71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>